<commit_message>
Creation of the database
</commit_message>
<xml_diff>
--- a/PlanningInitial.xlsx
+++ b/PlanningInitial.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/tdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74CDBF7F-8B51-4C18-8B73-98F4493994BA}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F26C031-CA41-4993-BDC7-B6DBCF276766}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24720" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Planning du travail de diplôme</t>
   </si>
@@ -79,6 +87,24 @@
   </si>
   <si>
     <t>Création du backend du logiciel</t>
+  </si>
+  <si>
+    <t>Rendu du rapport intermédiaire + poster</t>
+  </si>
+  <si>
+    <t>Rendu version intermédiaire du résumé et de l'abstract</t>
+  </si>
+  <si>
+    <t>Rendu travail</t>
+  </si>
+  <si>
+    <t>Création du poster</t>
+  </si>
+  <si>
+    <t>Implementation des mindmap</t>
+  </si>
+  <si>
+    <t>Implémentation du gantt</t>
   </si>
 </sst>
 </file>
@@ -118,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -126,25 +152,229 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,201 +656,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="C3" s="15">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="9">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -631,6 +974,15 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Creation and documentation of mockups
</commit_message>
<xml_diff>
--- a/PlanningInitial.xlsx
+++ b/PlanningInitial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/tdd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F26C031-CA41-4993-BDC7-B6DBCF276766}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AA83E00-7690-42D9-82DD-01861AC97A8D}"/>
   <bookViews>
-    <workbookView xWindow="-24720" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Planning du travail de diplôme</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Implémentation du gantt</t>
+  </si>
+  <si>
+    <t>Evaluation Intermédiaire 01</t>
+  </si>
+  <si>
+    <t>Evaluation Intermédiaire 02</t>
+  </si>
+  <si>
+    <t>Evaluation Intermédiaire 03</t>
+  </si>
+  <si>
+    <t>Jalon</t>
   </si>
 </sst>
 </file>
@@ -340,15 +352,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,6 +378,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,46 +683,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>18</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -720,10 +732,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -733,10 +745,10 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -746,10 +758,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -759,10 +771,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -772,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -785,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -798,10 +810,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -811,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -824,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -837,10 +849,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -850,10 +862,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -863,10 +875,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -876,10 +888,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="9"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -889,100 +901,85 @@
         <v>2</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="9"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>16</v>
+      <c r="A18" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="9">
-        <v>43958</v>
+      <c r="E18" s="6">
+        <v>43945</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>17</v>
+      <c r="A19" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="9">
+      <c r="E19" s="6">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6">
+        <v>43959</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>18</v>
-      </c>
-      <c r="B20" s="12" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10">
         <v>43990</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Icons and Started Poster
</commit_message>
<xml_diff>
--- a/PlanningInitial.xlsx
+++ b/PlanningInitial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AA83E00-7690-42D9-82DD-01861AC97A8D}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A825D518-C2AE-4BF5-A84F-26D5596EA91B}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -671,7 +671,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,9 @@
       <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,7 +746,9 @@
       <c r="C5" s="4">
         <v>0.5</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,7 +761,9 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>0.25</v>
+      </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>